<commit_message>
Project Update Till 100424
</commit_message>
<xml_diff>
--- a/Excel/Delivery/OTIF/Export.xlsx
+++ b/Excel/Delivery/OTIF/Export.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\GitHub\Mahle-dashboard\Excel\Delivery\OTIF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.52.95.143\Mahle-dashboard\Excel\Delivery\OTIF\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6E20CB-0A93-46CB-8422-715F6E126357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19635" windowHeight="8235" activeTab="2"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -38,9 +39,6 @@
     <t>Week</t>
   </si>
   <si>
-    <t>2023-01</t>
-  </si>
-  <si>
     <t>W1</t>
   </si>
   <si>
@@ -53,47 +51,26 @@
     <t>W4</t>
   </si>
   <si>
-    <t>2023-02</t>
+    <t>2024-01</t>
   </si>
   <si>
-    <t>2023-03</t>
+    <t>2024-02</t>
   </si>
   <si>
-    <t>2023-04</t>
+    <t>2024-03</t>
   </si>
   <si>
-    <t>2023-05</t>
-  </si>
-  <si>
-    <t>2023-06</t>
-  </si>
-  <si>
-    <t>2023-07</t>
-  </si>
-  <si>
-    <t>2023-08</t>
-  </si>
-  <si>
-    <t>2023-09</t>
-  </si>
-  <si>
-    <t>2023-10</t>
-  </si>
-  <si>
-    <t>2023-11</t>
-  </si>
-  <si>
-    <t>2023-12</t>
+    <t>2024-04</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,15 +80,49 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -134,26 +145,38 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -425,17 +448,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C345"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C347"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <pane ySplit="1" topLeftCell="A331" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A347" sqref="A347"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7265625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -450,1677 +473,1677 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="4">
+      <c r="A2" s="3">
         <v>44927</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>44928</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>44929</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>44930</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>44931</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>44932</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>44933</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>44934</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>44935</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>44936</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>44937</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>44938</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>44939</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="4">
+      <c r="A15" s="3">
         <v>44940</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="4">
+      <c r="A16" s="3">
         <v>44941</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="4">
+      <c r="A17" s="3">
         <v>44942</v>
       </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="4">
+      <c r="A18" s="3">
         <v>44943</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="4">
+      <c r="A19" s="3">
         <v>44944</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="4">
+      <c r="A20" s="3">
         <v>44945</v>
       </c>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="4">
+      <c r="A21" s="3">
         <v>44946</v>
       </c>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="4">
+      <c r="A22" s="3">
         <v>44947</v>
       </c>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="4">
+      <c r="A23" s="3">
         <v>44948</v>
       </c>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="4">
+      <c r="A24" s="3">
         <v>44949</v>
       </c>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="4">
+      <c r="A25" s="3">
         <v>44950</v>
       </c>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="4">
+      <c r="A26" s="3">
         <v>44951</v>
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="4">
+      <c r="A27" s="3">
         <v>44952</v>
       </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="4">
+      <c r="A28" s="3">
         <v>44953</v>
       </c>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="4">
+      <c r="A29" s="3">
         <v>44954</v>
       </c>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="4">
+      <c r="A30" s="3">
         <v>44955</v>
       </c>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" s="4">
+      <c r="A31" s="3">
         <v>44956</v>
       </c>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" s="4">
+      <c r="A32" s="3">
         <v>44957</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="4">
+      <c r="A33" s="3">
         <v>44958</v>
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="4">
+      <c r="A34" s="3">
         <v>44959</v>
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="4">
+      <c r="A35" s="3">
         <v>44960</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="4">
+      <c r="A36" s="3">
         <v>44961</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="4">
+      <c r="A37" s="3">
         <v>44962</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="4">
+      <c r="A38" s="3">
         <v>44963</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="4">
+      <c r="A39" s="3">
         <v>44964</v>
       </c>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" s="4">
+      <c r="A40" s="3">
         <v>44965</v>
       </c>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="4">
+      <c r="A41" s="3">
         <v>44966</v>
       </c>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42" s="4">
+      <c r="A42" s="3">
         <v>44967</v>
       </c>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43" s="4">
+      <c r="A43" s="3">
         <v>44968</v>
       </c>
     </row>
     <row r="44" spans="1:1">
-      <c r="A44" s="4">
+      <c r="A44" s="3">
         <v>44969</v>
       </c>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45" s="4">
+      <c r="A45" s="3">
         <v>44970</v>
       </c>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46" s="4">
+      <c r="A46" s="3">
         <v>44971</v>
       </c>
     </row>
     <row r="47" spans="1:1">
-      <c r="A47" s="4">
+      <c r="A47" s="3">
         <v>44972</v>
       </c>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48" s="4">
+      <c r="A48" s="3">
         <v>44973</v>
       </c>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49" s="4">
+      <c r="A49" s="3">
         <v>44974</v>
       </c>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="4">
+      <c r="A50" s="3">
         <v>44975</v>
       </c>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="4">
+      <c r="A51" s="3">
         <v>44976</v>
       </c>
     </row>
     <row r="52" spans="1:1">
-      <c r="A52" s="4">
+      <c r="A52" s="3">
         <v>44977</v>
       </c>
     </row>
     <row r="53" spans="1:1">
-      <c r="A53" s="4">
+      <c r="A53" s="3">
         <v>44978</v>
       </c>
     </row>
     <row r="54" spans="1:1">
-      <c r="A54" s="4">
+      <c r="A54" s="3">
         <v>44979</v>
       </c>
     </row>
     <row r="55" spans="1:1">
-      <c r="A55" s="4">
+      <c r="A55" s="3">
         <v>44980</v>
       </c>
     </row>
     <row r="56" spans="1:1">
-      <c r="A56" s="4">
+      <c r="A56" s="3">
         <v>44981</v>
       </c>
     </row>
     <row r="57" spans="1:1">
-      <c r="A57" s="4">
+      <c r="A57" s="3">
         <v>44982</v>
       </c>
     </row>
     <row r="58" spans="1:1">
-      <c r="A58" s="4">
+      <c r="A58" s="3">
         <v>44983</v>
       </c>
     </row>
     <row r="59" spans="1:1">
-      <c r="A59" s="4">
+      <c r="A59" s="3">
         <v>44984</v>
       </c>
     </row>
     <row r="60" spans="1:1">
-      <c r="A60" s="4">
+      <c r="A60" s="3">
         <v>44985</v>
       </c>
     </row>
     <row r="61" spans="1:1">
-      <c r="A61" s="4">
+      <c r="A61" s="3">
         <v>44986</v>
       </c>
     </row>
     <row r="62" spans="1:1">
-      <c r="A62" s="4">
+      <c r="A62" s="3">
         <v>44987</v>
       </c>
     </row>
     <row r="63" spans="1:1">
-      <c r="A63" s="4">
+      <c r="A63" s="3">
         <v>44988</v>
       </c>
     </row>
     <row r="64" spans="1:1">
-      <c r="A64" s="4">
+      <c r="A64" s="3">
         <v>44989</v>
       </c>
     </row>
     <row r="65" spans="1:1">
-      <c r="A65" s="4">
+      <c r="A65" s="3">
         <v>44990</v>
       </c>
     </row>
     <row r="66" spans="1:1">
-      <c r="A66" s="4">
+      <c r="A66" s="3">
         <v>44991</v>
       </c>
     </row>
     <row r="67" spans="1:1">
-      <c r="A67" s="4">
+      <c r="A67" s="3">
         <v>44992</v>
       </c>
     </row>
     <row r="68" spans="1:1">
-      <c r="A68" s="4">
+      <c r="A68" s="3">
         <v>44993</v>
       </c>
     </row>
     <row r="69" spans="1:1">
-      <c r="A69" s="4">
+      <c r="A69" s="3">
         <v>44994</v>
       </c>
     </row>
     <row r="70" spans="1:1">
-      <c r="A70" s="4">
+      <c r="A70" s="3">
         <v>44995</v>
       </c>
     </row>
     <row r="71" spans="1:1">
-      <c r="A71" s="4">
+      <c r="A71" s="3">
         <v>44996</v>
       </c>
     </row>
     <row r="72" spans="1:1">
-      <c r="A72" s="4">
+      <c r="A72" s="3">
         <v>44997</v>
       </c>
     </row>
     <row r="73" spans="1:1">
-      <c r="A73" s="4">
+      <c r="A73" s="3">
         <v>44998</v>
       </c>
     </row>
     <row r="74" spans="1:1">
-      <c r="A74" s="4">
+      <c r="A74" s="3">
         <v>44999</v>
       </c>
     </row>
     <row r="75" spans="1:1">
-      <c r="A75" s="4">
+      <c r="A75" s="3">
         <v>45000</v>
       </c>
     </row>
     <row r="76" spans="1:1">
-      <c r="A76" s="4">
+      <c r="A76" s="3">
         <v>45001</v>
       </c>
     </row>
     <row r="77" spans="1:1">
-      <c r="A77" s="4">
+      <c r="A77" s="3">
         <v>45002</v>
       </c>
     </row>
     <row r="78" spans="1:1">
-      <c r="A78" s="4">
+      <c r="A78" s="3">
         <v>45003</v>
       </c>
     </row>
     <row r="79" spans="1:1">
-      <c r="A79" s="4">
+      <c r="A79" s="3">
         <v>45004</v>
       </c>
     </row>
     <row r="80" spans="1:1">
-      <c r="A80" s="4">
+      <c r="A80" s="3">
         <v>45005</v>
       </c>
     </row>
     <row r="81" spans="1:1">
-      <c r="A81" s="4">
+      <c r="A81" s="3">
         <v>45006</v>
       </c>
     </row>
     <row r="82" spans="1:1">
-      <c r="A82" s="4">
+      <c r="A82" s="3">
         <v>45007</v>
       </c>
     </row>
     <row r="83" spans="1:1">
-      <c r="A83" s="4">
+      <c r="A83" s="3">
         <v>45008</v>
       </c>
     </row>
     <row r="84" spans="1:1">
-      <c r="A84" s="4">
+      <c r="A84" s="3">
         <v>45009</v>
       </c>
     </row>
     <row r="85" spans="1:1">
-      <c r="A85" s="4">
+      <c r="A85" s="3">
         <v>45010</v>
       </c>
     </row>
     <row r="86" spans="1:1">
-      <c r="A86" s="4">
+      <c r="A86" s="3">
         <v>45011</v>
       </c>
     </row>
     <row r="87" spans="1:1">
-      <c r="A87" s="4">
+      <c r="A87" s="3">
         <v>45012</v>
       </c>
     </row>
     <row r="88" spans="1:1">
-      <c r="A88" s="4">
+      <c r="A88" s="3">
         <v>45013</v>
       </c>
     </row>
     <row r="89" spans="1:1">
-      <c r="A89" s="4">
+      <c r="A89" s="3">
         <v>45014</v>
       </c>
     </row>
     <row r="90" spans="1:1">
-      <c r="A90" s="4">
+      <c r="A90" s="3">
         <v>45015</v>
       </c>
     </row>
     <row r="91" spans="1:1">
-      <c r="A91" s="4">
+      <c r="A91" s="3">
         <v>45016</v>
       </c>
     </row>
     <row r="92" spans="1:1">
-      <c r="A92" s="4">
+      <c r="A92" s="3">
         <v>45017</v>
       </c>
     </row>
     <row r="93" spans="1:1">
-      <c r="A93" s="4">
+      <c r="A93" s="3">
         <v>45018</v>
       </c>
     </row>
     <row r="94" spans="1:1">
-      <c r="A94" s="4">
+      <c r="A94" s="3">
         <v>45019</v>
       </c>
     </row>
     <row r="95" spans="1:1">
-      <c r="A95" s="4">
+      <c r="A95" s="3">
         <v>45020</v>
       </c>
     </row>
     <row r="96" spans="1:1">
-      <c r="A96" s="4">
+      <c r="A96" s="3">
         <v>45021</v>
       </c>
     </row>
     <row r="97" spans="1:1">
-      <c r="A97" s="4">
+      <c r="A97" s="3">
         <v>45022</v>
       </c>
     </row>
     <row r="98" spans="1:1">
-      <c r="A98" s="4">
+      <c r="A98" s="3">
         <v>45023</v>
       </c>
     </row>
     <row r="99" spans="1:1">
-      <c r="A99" s="4">
+      <c r="A99" s="3">
         <v>45024</v>
       </c>
     </row>
     <row r="100" spans="1:1">
-      <c r="A100" s="4">
+      <c r="A100" s="3">
         <v>45025</v>
       </c>
     </row>
     <row r="101" spans="1:1">
-      <c r="A101" s="4">
+      <c r="A101" s="3">
         <v>45026</v>
       </c>
     </row>
     <row r="102" spans="1:1">
-      <c r="A102" s="4">
+      <c r="A102" s="3">
         <v>45027</v>
       </c>
     </row>
     <row r="103" spans="1:1">
-      <c r="A103" s="4">
+      <c r="A103" s="3">
         <v>45028</v>
       </c>
     </row>
     <row r="104" spans="1:1">
-      <c r="A104" s="4">
+      <c r="A104" s="3">
         <v>45029</v>
       </c>
     </row>
     <row r="105" spans="1:1">
-      <c r="A105" s="4">
+      <c r="A105" s="3">
         <v>45030</v>
       </c>
     </row>
     <row r="106" spans="1:1">
-      <c r="A106" s="4">
+      <c r="A106" s="3">
         <v>45031</v>
       </c>
     </row>
     <row r="107" spans="1:1">
-      <c r="A107" s="4">
+      <c r="A107" s="3">
         <v>45032</v>
       </c>
     </row>
     <row r="108" spans="1:1">
-      <c r="A108" s="4">
+      <c r="A108" s="3">
         <v>45033</v>
       </c>
     </row>
     <row r="109" spans="1:1">
-      <c r="A109" s="4">
+      <c r="A109" s="3">
         <v>45034</v>
       </c>
     </row>
     <row r="110" spans="1:1">
-      <c r="A110" s="4">
+      <c r="A110" s="3">
         <v>45035</v>
       </c>
     </row>
     <row r="111" spans="1:1">
-      <c r="A111" s="4">
+      <c r="A111" s="3">
         <v>45036</v>
       </c>
     </row>
     <row r="112" spans="1:1">
-      <c r="A112" s="4">
+      <c r="A112" s="3">
         <v>45037</v>
       </c>
     </row>
     <row r="113" spans="1:1">
-      <c r="A113" s="4">
+      <c r="A113" s="3">
         <v>45038</v>
       </c>
     </row>
     <row r="114" spans="1:1">
-      <c r="A114" s="4">
+      <c r="A114" s="3">
         <v>45039</v>
       </c>
     </row>
     <row r="115" spans="1:1">
-      <c r="A115" s="4">
+      <c r="A115" s="3">
         <v>45040</v>
       </c>
     </row>
     <row r="116" spans="1:1">
-      <c r="A116" s="4">
+      <c r="A116" s="3">
         <v>45041</v>
       </c>
     </row>
     <row r="117" spans="1:1">
-      <c r="A117" s="4">
+      <c r="A117" s="3">
         <v>45042</v>
       </c>
     </row>
     <row r="118" spans="1:1">
-      <c r="A118" s="4">
+      <c r="A118" s="3">
         <v>45043</v>
       </c>
     </row>
     <row r="119" spans="1:1">
-      <c r="A119" s="4">
+      <c r="A119" s="3">
         <v>45044</v>
       </c>
     </row>
     <row r="120" spans="1:1">
-      <c r="A120" s="4">
+      <c r="A120" s="3">
         <v>45045</v>
       </c>
     </row>
     <row r="121" spans="1:1">
-      <c r="A121" s="4">
+      <c r="A121" s="3">
         <v>45046</v>
       </c>
     </row>
     <row r="122" spans="1:1">
-      <c r="A122" s="4">
+      <c r="A122" s="3">
         <v>45047</v>
       </c>
     </row>
     <row r="123" spans="1:1">
-      <c r="A123" s="4">
+      <c r="A123" s="3">
         <v>45048</v>
       </c>
     </row>
     <row r="124" spans="1:1">
-      <c r="A124" s="4">
+      <c r="A124" s="3">
         <v>45049</v>
       </c>
     </row>
     <row r="125" spans="1:1">
-      <c r="A125" s="4">
+      <c r="A125" s="3">
         <v>45050</v>
       </c>
     </row>
     <row r="126" spans="1:1">
-      <c r="A126" s="4">
+      <c r="A126" s="3">
         <v>45051</v>
       </c>
     </row>
     <row r="127" spans="1:1">
-      <c r="A127" s="4">
+      <c r="A127" s="3">
         <v>45052</v>
       </c>
     </row>
     <row r="128" spans="1:1">
-      <c r="A128" s="4">
+      <c r="A128" s="3">
         <v>45053</v>
       </c>
     </row>
     <row r="129" spans="1:1">
-      <c r="A129" s="4">
+      <c r="A129" s="3">
         <v>45054</v>
       </c>
     </row>
     <row r="130" spans="1:1">
-      <c r="A130" s="4">
+      <c r="A130" s="3">
         <v>45055</v>
       </c>
     </row>
     <row r="131" spans="1:1">
-      <c r="A131" s="4">
+      <c r="A131" s="3">
         <v>45056</v>
       </c>
     </row>
     <row r="132" spans="1:1">
-      <c r="A132" s="4">
+      <c r="A132" s="3">
         <v>45057</v>
       </c>
     </row>
     <row r="133" spans="1:1">
-      <c r="A133" s="4">
+      <c r="A133" s="3">
         <v>45058</v>
       </c>
     </row>
     <row r="134" spans="1:1">
-      <c r="A134" s="4">
+      <c r="A134" s="3">
         <v>45059</v>
       </c>
     </row>
     <row r="135" spans="1:1">
-      <c r="A135" s="4">
+      <c r="A135" s="3">
         <v>45060</v>
       </c>
     </row>
     <row r="136" spans="1:1">
-      <c r="A136" s="4">
+      <c r="A136" s="3">
         <v>45061</v>
       </c>
     </row>
     <row r="137" spans="1:1">
-      <c r="A137" s="4">
+      <c r="A137" s="3">
         <v>45062</v>
       </c>
     </row>
     <row r="138" spans="1:1">
-      <c r="A138" s="4">
+      <c r="A138" s="3">
         <v>45063</v>
       </c>
     </row>
     <row r="139" spans="1:1">
-      <c r="A139" s="4">
+      <c r="A139" s="3">
         <v>45064</v>
       </c>
     </row>
     <row r="140" spans="1:1">
-      <c r="A140" s="4">
+      <c r="A140" s="3">
         <v>45065</v>
       </c>
     </row>
     <row r="141" spans="1:1">
-      <c r="A141" s="4">
+      <c r="A141" s="3">
         <v>45066</v>
       </c>
     </row>
     <row r="142" spans="1:1">
-      <c r="A142" s="4">
+      <c r="A142" s="3">
         <v>45067</v>
       </c>
     </row>
     <row r="143" spans="1:1">
-      <c r="A143" s="4">
+      <c r="A143" s="3">
         <v>45068</v>
       </c>
     </row>
     <row r="144" spans="1:1">
-      <c r="A144" s="4">
+      <c r="A144" s="3">
         <v>45069</v>
       </c>
     </row>
     <row r="145" spans="1:1">
-      <c r="A145" s="4">
+      <c r="A145" s="3">
         <v>45070</v>
       </c>
     </row>
     <row r="146" spans="1:1">
-      <c r="A146" s="4">
+      <c r="A146" s="3">
         <v>45071</v>
       </c>
     </row>
     <row r="147" spans="1:1">
-      <c r="A147" s="4">
+      <c r="A147" s="3">
         <v>45072</v>
       </c>
     </row>
     <row r="148" spans="1:1">
-      <c r="A148" s="4">
+      <c r="A148" s="3">
         <v>45073</v>
       </c>
     </row>
     <row r="149" spans="1:1">
-      <c r="A149" s="4">
+      <c r="A149" s="3">
         <v>45074</v>
       </c>
     </row>
     <row r="150" spans="1:1">
-      <c r="A150" s="4">
+      <c r="A150" s="3">
         <v>45075</v>
       </c>
     </row>
     <row r="151" spans="1:1">
-      <c r="A151" s="4">
+      <c r="A151" s="3">
         <v>45076</v>
       </c>
     </row>
     <row r="152" spans="1:1">
-      <c r="A152" s="4">
+      <c r="A152" s="3">
         <v>45077</v>
       </c>
     </row>
     <row r="153" spans="1:1">
-      <c r="A153" s="4">
+      <c r="A153" s="3">
         <v>45078</v>
       </c>
     </row>
     <row r="154" spans="1:1">
-      <c r="A154" s="4">
+      <c r="A154" s="3">
         <v>45079</v>
       </c>
     </row>
     <row r="155" spans="1:1">
-      <c r="A155" s="4">
+      <c r="A155" s="3">
         <v>45080</v>
       </c>
     </row>
     <row r="156" spans="1:1">
-      <c r="A156" s="4">
+      <c r="A156" s="3">
         <v>45081</v>
       </c>
     </row>
     <row r="157" spans="1:1">
-      <c r="A157" s="4">
+      <c r="A157" s="3">
         <v>45082</v>
       </c>
     </row>
     <row r="158" spans="1:1">
-      <c r="A158" s="4">
+      <c r="A158" s="3">
         <v>45083</v>
       </c>
     </row>
     <row r="159" spans="1:1">
-      <c r="A159" s="4">
+      <c r="A159" s="3">
         <v>45084</v>
       </c>
     </row>
     <row r="160" spans="1:1">
-      <c r="A160" s="4">
+      <c r="A160" s="3">
         <v>45085</v>
       </c>
     </row>
     <row r="161" spans="1:1">
-      <c r="A161" s="4">
+      <c r="A161" s="3">
         <v>45086</v>
       </c>
     </row>
     <row r="162" spans="1:1">
-      <c r="A162" s="4">
+      <c r="A162" s="3">
         <v>45087</v>
       </c>
     </row>
     <row r="163" spans="1:1">
-      <c r="A163" s="4">
+      <c r="A163" s="3">
         <v>45088</v>
       </c>
     </row>
     <row r="164" spans="1:1">
-      <c r="A164" s="4">
+      <c r="A164" s="3">
         <v>45089</v>
       </c>
     </row>
     <row r="165" spans="1:1">
-      <c r="A165" s="4">
+      <c r="A165" s="3">
         <v>45090</v>
       </c>
     </row>
     <row r="166" spans="1:1">
-      <c r="A166" s="4">
+      <c r="A166" s="3">
         <v>45091</v>
       </c>
     </row>
     <row r="167" spans="1:1">
-      <c r="A167" s="4">
+      <c r="A167" s="3">
         <v>45092</v>
       </c>
     </row>
     <row r="168" spans="1:1">
-      <c r="A168" s="4">
+      <c r="A168" s="3">
         <v>45093</v>
       </c>
     </row>
     <row r="169" spans="1:1">
-      <c r="A169" s="4">
+      <c r="A169" s="3">
         <v>45094</v>
       </c>
     </row>
     <row r="170" spans="1:1">
-      <c r="A170" s="4">
+      <c r="A170" s="3">
         <v>45095</v>
       </c>
     </row>
     <row r="171" spans="1:1">
-      <c r="A171" s="4">
+      <c r="A171" s="3">
         <v>45096</v>
       </c>
     </row>
     <row r="172" spans="1:1">
-      <c r="A172" s="4">
+      <c r="A172" s="3">
         <v>45097</v>
       </c>
     </row>
     <row r="173" spans="1:1">
-      <c r="A173" s="4">
+      <c r="A173" s="3">
         <v>45098</v>
       </c>
     </row>
     <row r="174" spans="1:1">
-      <c r="A174" s="4">
+      <c r="A174" s="3">
         <v>45099</v>
       </c>
     </row>
     <row r="175" spans="1:1">
-      <c r="A175" s="4">
+      <c r="A175" s="3">
         <v>45100</v>
       </c>
     </row>
     <row r="176" spans="1:1">
-      <c r="A176" s="4">
+      <c r="A176" s="3">
         <v>45101</v>
       </c>
     </row>
     <row r="177" spans="1:1">
-      <c r="A177" s="4">
+      <c r="A177" s="3">
         <v>45102</v>
       </c>
     </row>
     <row r="178" spans="1:1">
-      <c r="A178" s="4">
+      <c r="A178" s="3">
         <v>45103</v>
       </c>
     </row>
     <row r="179" spans="1:1">
-      <c r="A179" s="4">
+      <c r="A179" s="3">
         <v>45104</v>
       </c>
     </row>
     <row r="180" spans="1:1">
-      <c r="A180" s="4">
+      <c r="A180" s="3">
         <v>45105</v>
       </c>
     </row>
     <row r="181" spans="1:1">
-      <c r="A181" s="4">
+      <c r="A181" s="3">
         <v>45106</v>
       </c>
     </row>
     <row r="182" spans="1:1">
-      <c r="A182" s="4">
+      <c r="A182" s="3">
         <v>45107</v>
       </c>
     </row>
     <row r="183" spans="1:1">
-      <c r="A183" s="4">
+      <c r="A183" s="3">
         <v>45108</v>
       </c>
     </row>
     <row r="184" spans="1:1">
-      <c r="A184" s="4">
+      <c r="A184" s="3">
         <v>45109</v>
       </c>
     </row>
     <row r="185" spans="1:1">
-      <c r="A185" s="4">
+      <c r="A185" s="3">
         <v>45110</v>
       </c>
     </row>
     <row r="186" spans="1:1">
-      <c r="A186" s="4">
+      <c r="A186" s="3">
         <v>45111</v>
       </c>
     </row>
     <row r="187" spans="1:1">
-      <c r="A187" s="4">
+      <c r="A187" s="3">
         <v>45112</v>
       </c>
     </row>
     <row r="188" spans="1:1">
-      <c r="A188" s="4">
+      <c r="A188" s="3">
         <v>45113</v>
       </c>
     </row>
     <row r="189" spans="1:1">
-      <c r="A189" s="4">
+      <c r="A189" s="3">
         <v>45114</v>
       </c>
     </row>
     <row r="190" spans="1:1">
-      <c r="A190" s="4">
+      <c r="A190" s="3">
         <v>45115</v>
       </c>
     </row>
     <row r="191" spans="1:1">
-      <c r="A191" s="4">
+      <c r="A191" s="3">
         <v>45116</v>
       </c>
     </row>
     <row r="192" spans="1:1">
-      <c r="A192" s="4">
+      <c r="A192" s="3">
         <v>45117</v>
       </c>
     </row>
     <row r="193" spans="1:1">
-      <c r="A193" s="4">
+      <c r="A193" s="3">
         <v>45118</v>
       </c>
     </row>
     <row r="194" spans="1:1">
-      <c r="A194" s="4">
+      <c r="A194" s="3">
         <v>45119</v>
       </c>
     </row>
     <row r="195" spans="1:1">
-      <c r="A195" s="4">
+      <c r="A195" s="3">
         <v>45120</v>
       </c>
     </row>
     <row r="196" spans="1:1">
-      <c r="A196" s="4">
+      <c r="A196" s="3">
         <v>45121</v>
       </c>
     </row>
     <row r="197" spans="1:1">
-      <c r="A197" s="4">
+      <c r="A197" s="3">
         <v>45122</v>
       </c>
     </row>
     <row r="198" spans="1:1">
-      <c r="A198" s="4">
+      <c r="A198" s="3">
         <v>45123</v>
       </c>
     </row>
     <row r="199" spans="1:1">
-      <c r="A199" s="4">
+      <c r="A199" s="3">
         <v>45124</v>
       </c>
     </row>
     <row r="200" spans="1:1">
-      <c r="A200" s="4">
+      <c r="A200" s="3">
         <v>45125</v>
       </c>
     </row>
     <row r="201" spans="1:1">
-      <c r="A201" s="4">
+      <c r="A201" s="3">
         <v>45126</v>
       </c>
     </row>
     <row r="202" spans="1:1">
-      <c r="A202" s="4">
+      <c r="A202" s="3">
         <v>45127</v>
       </c>
     </row>
     <row r="203" spans="1:1">
-      <c r="A203" s="4">
+      <c r="A203" s="3">
         <v>45128</v>
       </c>
     </row>
     <row r="204" spans="1:1">
-      <c r="A204" s="4">
+      <c r="A204" s="3">
         <v>45129</v>
       </c>
     </row>
     <row r="205" spans="1:1">
-      <c r="A205" s="4">
+      <c r="A205" s="3">
         <v>45130</v>
       </c>
     </row>
     <row r="206" spans="1:1">
-      <c r="A206" s="4">
+      <c r="A206" s="3">
         <v>45131</v>
       </c>
     </row>
     <row r="207" spans="1:1">
-      <c r="A207" s="4">
+      <c r="A207" s="3">
         <v>45132</v>
       </c>
     </row>
     <row r="208" spans="1:1">
-      <c r="A208" s="4">
+      <c r="A208" s="3">
         <v>45133</v>
       </c>
     </row>
     <row r="209" spans="1:1">
-      <c r="A209" s="4">
+      <c r="A209" s="3">
         <v>45134</v>
       </c>
     </row>
     <row r="210" spans="1:1">
-      <c r="A210" s="4">
+      <c r="A210" s="3">
         <v>45135</v>
       </c>
     </row>
     <row r="211" spans="1:1">
-      <c r="A211" s="4">
+      <c r="A211" s="3">
         <v>45136</v>
       </c>
     </row>
     <row r="212" spans="1:1">
-      <c r="A212" s="4">
+      <c r="A212" s="3">
         <v>45137</v>
       </c>
     </row>
     <row r="213" spans="1:1">
-      <c r="A213" s="4">
+      <c r="A213" s="3">
         <v>45138</v>
       </c>
     </row>
     <row r="214" spans="1:1">
-      <c r="A214" s="4">
+      <c r="A214" s="3">
         <v>45139</v>
       </c>
     </row>
     <row r="215" spans="1:1">
-      <c r="A215" s="4">
+      <c r="A215" s="3">
         <v>45140</v>
       </c>
     </row>
     <row r="216" spans="1:1">
-      <c r="A216" s="4">
+      <c r="A216" s="3">
         <v>45141</v>
       </c>
     </row>
     <row r="217" spans="1:1">
-      <c r="A217" s="4">
+      <c r="A217" s="3">
         <v>45142</v>
       </c>
     </row>
     <row r="218" spans="1:1">
-      <c r="A218" s="4">
+      <c r="A218" s="3">
         <v>45143</v>
       </c>
     </row>
     <row r="219" spans="1:1">
-      <c r="A219" s="4">
+      <c r="A219" s="3">
         <v>45144</v>
       </c>
     </row>
     <row r="220" spans="1:1">
-      <c r="A220" s="4">
+      <c r="A220" s="3">
         <v>45145</v>
       </c>
     </row>
     <row r="221" spans="1:1">
-      <c r="A221" s="4">
+      <c r="A221" s="3">
         <v>45146</v>
       </c>
     </row>
     <row r="222" spans="1:1">
-      <c r="A222" s="4">
+      <c r="A222" s="3">
         <v>45147</v>
       </c>
     </row>
     <row r="223" spans="1:1">
-      <c r="A223" s="4">
+      <c r="A223" s="3">
         <v>45148</v>
       </c>
     </row>
     <row r="224" spans="1:1">
-      <c r="A224" s="4">
+      <c r="A224" s="3">
         <v>45149</v>
       </c>
     </row>
     <row r="225" spans="1:1">
-      <c r="A225" s="4">
+      <c r="A225" s="3">
         <v>45150</v>
       </c>
     </row>
     <row r="226" spans="1:1">
-      <c r="A226" s="4">
+      <c r="A226" s="3">
         <v>45151</v>
       </c>
     </row>
     <row r="227" spans="1:1">
-      <c r="A227" s="4">
+      <c r="A227" s="3">
         <v>45152</v>
       </c>
     </row>
     <row r="228" spans="1:1">
-      <c r="A228" s="4">
+      <c r="A228" s="3">
         <v>45153</v>
       </c>
     </row>
     <row r="229" spans="1:1">
-      <c r="A229" s="4">
+      <c r="A229" s="3">
         <v>45154</v>
       </c>
     </row>
     <row r="230" spans="1:1">
-      <c r="A230" s="4">
+      <c r="A230" s="3">
         <v>45155</v>
       </c>
     </row>
     <row r="231" spans="1:1">
-      <c r="A231" s="4">
+      <c r="A231" s="3">
         <v>45156</v>
       </c>
     </row>
     <row r="232" spans="1:1">
-      <c r="A232" s="4">
+      <c r="A232" s="3">
         <v>45157</v>
       </c>
     </row>
     <row r="233" spans="1:1">
-      <c r="A233" s="4">
+      <c r="A233" s="3">
         <v>45158</v>
       </c>
     </row>
     <row r="234" spans="1:1">
-      <c r="A234" s="4">
+      <c r="A234" s="3">
         <v>45159</v>
       </c>
     </row>
     <row r="235" spans="1:1">
-      <c r="A235" s="4">
+      <c r="A235" s="3">
         <v>45160</v>
       </c>
     </row>
     <row r="236" spans="1:1">
-      <c r="A236" s="4">
+      <c r="A236" s="3">
         <v>45161</v>
       </c>
     </row>
     <row r="237" spans="1:1">
-      <c r="A237" s="4">
+      <c r="A237" s="3">
         <v>45162</v>
       </c>
     </row>
     <row r="238" spans="1:1">
-      <c r="A238" s="4">
+      <c r="A238" s="3">
         <v>45163</v>
       </c>
     </row>
     <row r="239" spans="1:1">
-      <c r="A239" s="4">
+      <c r="A239" s="3">
         <v>45164</v>
       </c>
     </row>
     <row r="240" spans="1:1">
-      <c r="A240" s="4">
+      <c r="A240" s="3">
         <v>45165</v>
       </c>
     </row>
     <row r="241" spans="1:1">
-      <c r="A241" s="4">
+      <c r="A241" s="3">
         <v>45166</v>
       </c>
     </row>
     <row r="242" spans="1:1">
-      <c r="A242" s="4">
+      <c r="A242" s="3">
         <v>45167</v>
       </c>
     </row>
     <row r="243" spans="1:1">
-      <c r="A243" s="4">
+      <c r="A243" s="3">
         <v>45168</v>
       </c>
     </row>
     <row r="244" spans="1:1">
-      <c r="A244" s="4">
+      <c r="A244" s="3">
         <v>45169</v>
       </c>
     </row>
     <row r="245" spans="1:1">
-      <c r="A245" s="4">
+      <c r="A245" s="3">
         <v>45170</v>
       </c>
     </row>
     <row r="246" spans="1:1">
-      <c r="A246" s="4">
+      <c r="A246" s="3">
         <v>45171</v>
       </c>
     </row>
     <row r="247" spans="1:1">
-      <c r="A247" s="4">
+      <c r="A247" s="3">
         <v>45172</v>
       </c>
     </row>
     <row r="248" spans="1:1">
-      <c r="A248" s="4">
+      <c r="A248" s="3">
         <v>45173</v>
       </c>
     </row>
     <row r="249" spans="1:1">
-      <c r="A249" s="4">
+      <c r="A249" s="3">
         <v>45174</v>
       </c>
     </row>
     <row r="250" spans="1:1">
-      <c r="A250" s="4">
+      <c r="A250" s="3">
         <v>45175</v>
       </c>
     </row>
     <row r="251" spans="1:1">
-      <c r="A251" s="4">
+      <c r="A251" s="3">
         <v>45176</v>
       </c>
     </row>
     <row r="252" spans="1:1">
-      <c r="A252" s="4">
+      <c r="A252" s="3">
         <v>45177</v>
       </c>
     </row>
     <row r="253" spans="1:1">
-      <c r="A253" s="4">
+      <c r="A253" s="3">
         <v>45178</v>
       </c>
     </row>
     <row r="254" spans="1:1">
-      <c r="A254" s="4">
+      <c r="A254" s="3">
         <v>45179</v>
       </c>
     </row>
     <row r="255" spans="1:1">
-      <c r="A255" s="4">
+      <c r="A255" s="3">
         <v>45180</v>
       </c>
     </row>
     <row r="256" spans="1:1">
-      <c r="A256" s="4">
+      <c r="A256" s="3">
         <v>45181</v>
       </c>
     </row>
     <row r="257" spans="1:1">
-      <c r="A257" s="4">
+      <c r="A257" s="3">
         <v>45182</v>
       </c>
     </row>
     <row r="258" spans="1:1">
-      <c r="A258" s="4">
+      <c r="A258" s="3">
         <v>45183</v>
       </c>
     </row>
     <row r="259" spans="1:1">
-      <c r="A259" s="4">
+      <c r="A259" s="3">
         <v>45184</v>
       </c>
     </row>
     <row r="260" spans="1:1">
-      <c r="A260" s="4">
+      <c r="A260" s="3">
         <v>45185</v>
       </c>
     </row>
     <row r="261" spans="1:1">
-      <c r="A261" s="4">
+      <c r="A261" s="3">
         <v>45186</v>
       </c>
     </row>
     <row r="262" spans="1:1">
-      <c r="A262" s="4">
+      <c r="A262" s="3">
         <v>45187</v>
       </c>
     </row>
     <row r="263" spans="1:1">
-      <c r="A263" s="4">
+      <c r="A263" s="3">
         <v>45188</v>
       </c>
     </row>
     <row r="264" spans="1:1">
-      <c r="A264" s="4">
+      <c r="A264" s="3">
         <v>45189</v>
       </c>
     </row>
     <row r="265" spans="1:1">
-      <c r="A265" s="4">
+      <c r="A265" s="3">
         <v>45190</v>
       </c>
     </row>
     <row r="266" spans="1:1">
-      <c r="A266" s="4">
+      <c r="A266" s="3">
         <v>45191</v>
       </c>
     </row>
     <row r="267" spans="1:1">
-      <c r="A267" s="4">
+      <c r="A267" s="3">
         <v>45192</v>
       </c>
     </row>
     <row r="268" spans="1:1">
-      <c r="A268" s="4">
+      <c r="A268" s="3">
         <v>45193</v>
       </c>
     </row>
     <row r="269" spans="1:1">
-      <c r="A269" s="4">
+      <c r="A269" s="3">
         <v>45194</v>
       </c>
     </row>
     <row r="270" spans="1:1">
-      <c r="A270" s="4">
+      <c r="A270" s="3">
         <v>45195</v>
       </c>
     </row>
     <row r="271" spans="1:1">
-      <c r="A271" s="4">
+      <c r="A271" s="3">
         <v>45196</v>
       </c>
     </row>
     <row r="272" spans="1:1">
-      <c r="A272" s="4">
+      <c r="A272" s="3">
         <v>45197</v>
       </c>
     </row>
     <row r="273" spans="1:1">
-      <c r="A273" s="4">
+      <c r="A273" s="3">
         <v>45198</v>
       </c>
     </row>
     <row r="274" spans="1:1">
-      <c r="A274" s="4">
+      <c r="A274" s="3">
         <v>45199</v>
       </c>
     </row>
     <row r="275" spans="1:1">
-      <c r="A275" s="4">
+      <c r="A275" s="3">
         <v>45200</v>
       </c>
     </row>
     <row r="276" spans="1:1">
-      <c r="A276" s="4">
+      <c r="A276" s="3">
         <v>45201</v>
       </c>
     </row>
     <row r="277" spans="1:1">
-      <c r="A277" s="4">
+      <c r="A277" s="3">
         <v>45202</v>
       </c>
     </row>
     <row r="278" spans="1:1">
-      <c r="A278" s="4">
+      <c r="A278" s="3">
         <v>45203</v>
       </c>
     </row>
     <row r="279" spans="1:1">
-      <c r="A279" s="4">
+      <c r="A279" s="3">
         <v>45204</v>
       </c>
     </row>
     <row r="280" spans="1:1">
-      <c r="A280" s="4">
+      <c r="A280" s="3">
         <v>45205</v>
       </c>
     </row>
     <row r="281" spans="1:1">
-      <c r="A281" s="4">
+      <c r="A281" s="3">
         <v>45206</v>
       </c>
     </row>
     <row r="282" spans="1:1">
-      <c r="A282" s="4">
+      <c r="A282" s="3">
         <v>45207</v>
       </c>
     </row>
     <row r="283" spans="1:1">
-      <c r="A283" s="4">
+      <c r="A283" s="3">
         <v>45208</v>
       </c>
     </row>
     <row r="284" spans="1:1">
-      <c r="A284" s="4">
+      <c r="A284" s="3">
         <v>45209</v>
       </c>
     </row>
     <row r="285" spans="1:1">
-      <c r="A285" s="4">
+      <c r="A285" s="3">
         <v>45210</v>
       </c>
     </row>
     <row r="286" spans="1:1">
-      <c r="A286" s="4">
+      <c r="A286" s="3">
         <v>45211</v>
       </c>
     </row>
     <row r="287" spans="1:1">
-      <c r="A287" s="4">
+      <c r="A287" s="3">
         <v>45212</v>
       </c>
     </row>
     <row r="288" spans="1:1">
-      <c r="A288" s="4">
+      <c r="A288" s="3">
         <v>45213</v>
       </c>
     </row>
     <row r="289" spans="1:1">
-      <c r="A289" s="4">
+      <c r="A289" s="3">
         <v>45214</v>
       </c>
     </row>
     <row r="290" spans="1:1">
-      <c r="A290" s="4">
+      <c r="A290" s="3">
         <v>45215</v>
       </c>
     </row>
     <row r="291" spans="1:1">
-      <c r="A291" s="4">
+      <c r="A291" s="3">
         <v>45216</v>
       </c>
     </row>
     <row r="292" spans="1:1">
-      <c r="A292" s="4">
+      <c r="A292" s="3">
         <v>45217</v>
       </c>
     </row>
     <row r="293" spans="1:1">
-      <c r="A293" s="4">
+      <c r="A293" s="3">
         <v>45218</v>
       </c>
     </row>
     <row r="294" spans="1:1">
-      <c r="A294" s="4">
+      <c r="A294" s="3">
         <v>45219</v>
       </c>
     </row>
     <row r="295" spans="1:1">
-      <c r="A295" s="4">
+      <c r="A295" s="3">
         <v>45220</v>
       </c>
     </row>
     <row r="296" spans="1:1">
-      <c r="A296" s="4">
+      <c r="A296" s="3">
         <v>45221</v>
       </c>
     </row>
     <row r="297" spans="1:1">
-      <c r="A297" s="4">
+      <c r="A297" s="3">
         <v>45222</v>
       </c>
     </row>
     <row r="298" spans="1:1">
-      <c r="A298" s="4">
+      <c r="A298" s="3">
         <v>45223</v>
       </c>
     </row>
     <row r="299" spans="1:1">
-      <c r="A299" s="4">
+      <c r="A299" s="3">
         <v>45224</v>
       </c>
     </row>
     <row r="300" spans="1:1">
-      <c r="A300" s="4">
+      <c r="A300" s="3">
         <v>45225</v>
       </c>
     </row>
     <row r="301" spans="1:1">
-      <c r="A301" s="4">
+      <c r="A301" s="3">
         <v>45226</v>
       </c>
     </row>
     <row r="302" spans="1:1">
-      <c r="A302" s="4">
+      <c r="A302" s="3">
         <v>45227</v>
       </c>
     </row>
     <row r="303" spans="1:1">
-      <c r="A303" s="4">
+      <c r="A303" s="3">
         <v>45228</v>
       </c>
     </row>
     <row r="304" spans="1:1">
-      <c r="A304" s="4">
+      <c r="A304" s="3">
         <v>45229</v>
       </c>
     </row>
     <row r="305" spans="1:1">
-      <c r="A305" s="4">
+      <c r="A305" s="3">
         <v>45230</v>
       </c>
     </row>
     <row r="306" spans="1:1">
-      <c r="A306" s="4">
+      <c r="A306" s="3">
         <v>45231</v>
       </c>
     </row>
     <row r="307" spans="1:1">
-      <c r="A307" s="4">
+      <c r="A307" s="3">
         <v>45232</v>
       </c>
     </row>
     <row r="308" spans="1:1">
-      <c r="A308" s="4">
+      <c r="A308" s="3">
         <v>45233</v>
       </c>
     </row>
     <row r="309" spans="1:1">
-      <c r="A309" s="4">
+      <c r="A309" s="3">
         <v>45234</v>
       </c>
     </row>
     <row r="310" spans="1:1">
-      <c r="A310" s="4">
+      <c r="A310" s="3">
         <v>45235</v>
       </c>
     </row>
     <row r="311" spans="1:1">
-      <c r="A311" s="4">
+      <c r="A311" s="3">
         <v>45236</v>
       </c>
     </row>
     <row r="312" spans="1:1">
-      <c r="A312" s="4">
+      <c r="A312" s="3">
         <v>45237</v>
       </c>
     </row>
     <row r="313" spans="1:1">
-      <c r="A313" s="4">
+      <c r="A313" s="3">
         <v>45238</v>
       </c>
     </row>
     <row r="314" spans="1:1">
-      <c r="A314" s="4">
+      <c r="A314" s="3">
         <v>45239</v>
       </c>
     </row>
     <row r="315" spans="1:1">
-      <c r="A315" s="4">
+      <c r="A315" s="3">
         <v>45240</v>
       </c>
     </row>
     <row r="316" spans="1:1">
-      <c r="A316" s="4">
+      <c r="A316" s="3">
         <v>45241</v>
       </c>
     </row>
     <row r="317" spans="1:1">
-      <c r="A317" s="4">
+      <c r="A317" s="3">
         <v>45242</v>
       </c>
     </row>
     <row r="318" spans="1:1">
-      <c r="A318" s="4">
+      <c r="A318" s="3">
         <v>45243</v>
       </c>
     </row>
     <row r="319" spans="1:1">
-      <c r="A319" s="4">
+      <c r="A319" s="3">
         <v>45244</v>
       </c>
     </row>
     <row r="320" spans="1:1">
-      <c r="A320" s="4">
+      <c r="A320" s="3">
         <v>45245</v>
       </c>
     </row>
     <row r="321" spans="1:3">
-      <c r="A321" s="4">
+      <c r="A321" s="3">
         <v>45246</v>
       </c>
     </row>
     <row r="322" spans="1:3">
-      <c r="A322" s="4">
+      <c r="A322" s="3">
         <v>45247</v>
       </c>
     </row>
     <row r="323" spans="1:3">
-      <c r="A323" s="4">
+      <c r="A323" s="3">
         <v>45248</v>
       </c>
     </row>
     <row r="324" spans="1:3">
-      <c r="A324" s="4">
+      <c r="A324" s="3">
         <v>45249</v>
       </c>
     </row>
     <row r="325" spans="1:3">
-      <c r="A325" s="4">
+      <c r="A325" s="3">
         <v>45250</v>
       </c>
     </row>
     <row r="326" spans="1:3">
-      <c r="A326" s="4">
+      <c r="A326" s="3">
         <v>45251</v>
       </c>
     </row>
     <row r="327" spans="1:3">
-      <c r="A327" s="4">
+      <c r="A327" s="3">
         <v>45252</v>
       </c>
     </row>
     <row r="328" spans="1:3">
-      <c r="A328" s="4">
+      <c r="A328" s="3">
         <v>45253</v>
       </c>
     </row>
     <row r="329" spans="1:3">
-      <c r="A329" s="4">
+      <c r="A329" s="3">
         <v>45254</v>
       </c>
     </row>
     <row r="330" spans="1:3">
-      <c r="A330" s="4">
+      <c r="A330" s="3">
         <v>45255</v>
       </c>
     </row>
     <row r="331" spans="1:3">
-      <c r="A331" s="4">
+      <c r="A331" s="3">
         <v>45256</v>
       </c>
     </row>
     <row r="332" spans="1:3">
-      <c r="A332" s="4">
+      <c r="A332" s="3">
         <v>45257</v>
       </c>
     </row>
     <row r="333" spans="1:3">
-      <c r="A333" s="4">
+      <c r="A333" s="3">
         <v>45258</v>
       </c>
     </row>
     <row r="334" spans="1:3">
-      <c r="A334" s="4">
+      <c r="A334" s="3">
         <v>45259</v>
       </c>
     </row>
     <row r="335" spans="1:3">
-      <c r="A335" s="4">
+      <c r="A335" s="3">
         <v>45260</v>
       </c>
     </row>
     <row r="336" spans="1:3">
-      <c r="A336" s="4">
+      <c r="A336" s="3">
         <v>45261</v>
       </c>
       <c r="B336">
@@ -2131,7 +2154,7 @@
       </c>
     </row>
     <row r="337" spans="1:3">
-      <c r="A337" s="4">
+      <c r="A337" s="3">
         <v>45262</v>
       </c>
       <c r="B337">
@@ -2142,7 +2165,7 @@
       </c>
     </row>
     <row r="338" spans="1:3">
-      <c r="A338" s="4">
+      <c r="A338" s="3">
         <v>45263</v>
       </c>
       <c r="B338">
@@ -2153,7 +2176,7 @@
       </c>
     </row>
     <row r="339" spans="1:3">
-      <c r="A339" s="4">
+      <c r="A339" s="3">
         <v>45264</v>
       </c>
       <c r="B339">
@@ -2164,7 +2187,7 @@
       </c>
     </row>
     <row r="340" spans="1:3">
-      <c r="A340" s="4">
+      <c r="A340" s="3">
         <v>45265</v>
       </c>
       <c r="B340">
@@ -2175,7 +2198,7 @@
       </c>
     </row>
     <row r="341" spans="1:3">
-      <c r="A341" s="4">
+      <c r="A341" s="3">
         <v>45266</v>
       </c>
       <c r="B341">
@@ -2186,7 +2209,7 @@
       </c>
     </row>
     <row r="342" spans="1:3">
-      <c r="A342" s="4">
+      <c r="A342" s="3">
         <v>45267</v>
       </c>
       <c r="B342">
@@ -2197,7 +2220,7 @@
       </c>
     </row>
     <row r="343" spans="1:3">
-      <c r="A343" s="4">
+      <c r="A343" s="3">
         <v>45268</v>
       </c>
       <c r="B343">
@@ -2208,7 +2231,7 @@
       </c>
     </row>
     <row r="344" spans="1:3">
-      <c r="A344" s="4">
+      <c r="A344" s="3">
         <v>45269</v>
       </c>
       <c r="B344">
@@ -2219,7 +2242,7 @@
       </c>
     </row>
     <row r="345" spans="1:3">
-      <c r="A345" s="4">
+      <c r="A345" s="3">
         <v>45270</v>
       </c>
       <c r="B345">
@@ -2229,21 +2252,40 @@
         <v>244</v>
       </c>
     </row>
+    <row r="346" spans="1:3">
+      <c r="A346" s="3">
+        <v>45292</v>
+      </c>
+      <c r="B346">
+        <v>100</v>
+      </c>
+      <c r="C346">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="347" spans="1:3">
+      <c r="A347" s="3">
+        <v>45293</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 MAHLE internal (CL2)</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -2260,516 +2302,197 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1">
+        <v>100</v>
+      </c>
+      <c r="D2" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
+      <c r="C3" s="1">
+        <v>100</v>
+      </c>
+      <c r="D3" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1">
+        <v>100</v>
+      </c>
+      <c r="D4" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1">
+        <v>100</v>
+      </c>
+      <c r="D5" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C6" s="1">
+        <v>100</v>
+      </c>
+      <c r="D6" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1">
+        <v>100</v>
+      </c>
+      <c r="D7" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
+      <c r="C8" s="1">
+        <v>100</v>
+      </c>
+      <c r="D8" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1">
+        <v>100</v>
+      </c>
+      <c r="D9" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C10" s="1">
+        <v>100</v>
+      </c>
+      <c r="D10" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1">
+        <v>100</v>
+      </c>
+      <c r="D11" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1">
+        <v>100</v>
+      </c>
+      <c r="D12" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="C13" s="1">
+        <v>100</v>
+      </c>
+      <c r="D13" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C46" s="1">
-        <v>123</v>
-      </c>
-      <c r="D46" s="1">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C47" s="1">
-        <v>124</v>
-      </c>
-      <c r="D47" s="1">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C48" s="1">
-        <v>125</v>
-      </c>
-      <c r="D48" s="1">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C49" s="1">
-        <v>126</v>
-      </c>
-      <c r="D49" s="1">
-        <v>459</v>
-      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 MAHLE internal (CL2)</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
@@ -2783,138 +2506,43 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
-        <v>5</v>
+      <c r="A2" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="B2" s="1">
-        <v>12</v>
+        <v>100</v>
       </c>
       <c r="C2">
-        <v>89</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1">
-        <v>13</v>
+        <v>100</v>
       </c>
       <c r="C3">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="1">
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="C4">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1">
-        <v>15</v>
-      </c>
-      <c r="C5">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="1">
-        <v>16</v>
-      </c>
-      <c r="C6">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="1">
-        <v>17</v>
-      </c>
-      <c r="C7">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="1">
-        <v>18</v>
-      </c>
-      <c r="C8">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="1">
-        <v>19</v>
-      </c>
-      <c r="C9">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="1">
-        <v>20</v>
-      </c>
-      <c r="C10">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="1">
-        <v>21</v>
-      </c>
-      <c r="C11">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="1">
-        <v>22</v>
-      </c>
-      <c r="C12">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="1">
-        <v>23</v>
-      </c>
-      <c r="C13">
         <v>100</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 MAHLE internal (CL2)</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>